<commit_message>
Update Hoi Dong Danh Gia Ket Qua
</commit_message>
<xml_diff>
--- a/Content/ExcelFiles/ListTeacher2.xlsx
+++ b/Content/ExcelFiles/ListTeacher2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KyThuat88\Documents\TranVietHoang_1621050401\ExcelFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33C4D593-DB99-4980-8283-DAEFA22D9783}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D510D8C-1AA0-4373-BD41-7982A26318DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A8A11DD1-21CB-4926-8D51-E69A41F06817}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
   <si>
     <t>MaGiangVien</t>
   </si>
@@ -124,13 +124,154 @@
   </si>
   <si>
     <t>nguyenthuhang@humg.edu.vn</t>
+  </si>
+  <si>
+    <t>0802-01</t>
+  </si>
+  <si>
+    <t>Phạm Quang</t>
+  </si>
+  <si>
+    <t>Hiển</t>
+  </si>
+  <si>
+    <t>Phạm Quang Hiển</t>
+  </si>
+  <si>
+    <t>phamquanghien@humg.edu.vn</t>
+  </si>
+  <si>
+    <t>0804-01</t>
+  </si>
+  <si>
+    <t>Phạm Thị</t>
+  </si>
+  <si>
+    <t>Nguyệt</t>
+  </si>
+  <si>
+    <t>Phạm Thị Nguyệt</t>
+  </si>
+  <si>
+    <t>phamthinguyet@humg.edu.vn</t>
+  </si>
+  <si>
+    <t>0806-01</t>
+  </si>
+  <si>
+    <t>Võ Thị Thu</t>
+  </si>
+  <si>
+    <t>Trang</t>
+  </si>
+  <si>
+    <t>Võ Thị Thu Trang</t>
+  </si>
+  <si>
+    <t>vothithutrang@humg.edu.vn</t>
+  </si>
+  <si>
+    <t>0807-01</t>
+  </si>
+  <si>
+    <t>Vũ Thị Kim</t>
+  </si>
+  <si>
+    <t>Liên</t>
+  </si>
+  <si>
+    <t>Vũ Thị Kim Liên</t>
+  </si>
+  <si>
+    <t>vuthikimlien@humg.edu.vn</t>
+  </si>
+  <si>
+    <t>0809-01</t>
+  </si>
+  <si>
+    <t>Hoàng Anh</t>
+  </si>
+  <si>
+    <t>Đức</t>
+  </si>
+  <si>
+    <t>Hoàng Anh Đức</t>
+  </si>
+  <si>
+    <t>hoanganhduc@humg.edu.vn</t>
+  </si>
+  <si>
+    <t>0801</t>
+  </si>
+  <si>
+    <t>Bộ môn Khoa học máy tính</t>
+  </si>
+  <si>
+    <t>0810-01</t>
+  </si>
+  <si>
+    <t>Lê Văn</t>
+  </si>
+  <si>
+    <t>Ngọc</t>
+  </si>
+  <si>
+    <t>Lê Văn Ngọc</t>
+  </si>
+  <si>
+    <t>levanngoc@humg.edu.vn</t>
+  </si>
+  <si>
+    <t>0811-01</t>
+  </si>
+  <si>
+    <t>Lê Hồng</t>
+  </si>
+  <si>
+    <t>Anh</t>
+  </si>
+  <si>
+    <t>Lê Hồng Anh</t>
+  </si>
+  <si>
+    <t>lehonganh@humg.edu.vn</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>0813-01</t>
+  </si>
+  <si>
+    <t>Nguyễn Duy</t>
+  </si>
+  <si>
+    <t>Huy</t>
+  </si>
+  <si>
+    <t>Nguyễn Duy Huy</t>
+  </si>
+  <si>
+    <t>nguyenduyhuy@humg.edu.vn</t>
+  </si>
+  <si>
+    <t>0814-01</t>
+  </si>
+  <si>
+    <t>Hưng</t>
+  </si>
+  <si>
+    <t>Lê Văn Hưng</t>
+  </si>
+  <si>
+    <t>levanghung@humg.edu.vn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +297,17 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="4">
@@ -206,7 +358,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -216,6 +368,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,14 +692,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70DD2FE-46D4-48F5-A7FB-B9FC9764A260}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="7" max="7" width="25.44140625" customWidth="1"/>
     <col min="8" max="8" width="28.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -573,11 +735,6 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
     </row>
     <row r="2" spans="1:19" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -610,11 +767,6 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
     </row>
     <row r="3" spans="1:19" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -647,11 +799,6 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
     </row>
     <row r="4" spans="1:19" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -684,11 +831,6 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
     </row>
     <row r="5" spans="1:19" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -721,11 +863,339 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="13">
+        <v>973876072</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="13">
+        <v>904170053</v>
+      </c>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="13">
+        <v>983888601</v>
+      </c>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+    </row>
+    <row r="9" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="13">
+        <v>984603666</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="13">
+        <v>914775545</v>
+      </c>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="13">
+        <v>986243482</v>
+      </c>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+    </row>
+    <row r="12" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="13">
+        <v>944555232</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+    </row>
+    <row r="13" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="13">
+        <v>966219991</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="15">
+        <v>833665555</v>
+      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -733,6 +1203,15 @@
     <hyperlink ref="E3" r:id="rId2" xr:uid="{B25D6609-3C29-4195-8EBE-1D71D681A2A7}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{44EABBDC-90E5-4694-936F-1265ADE564C3}"/>
     <hyperlink ref="E5" r:id="rId4" xr:uid="{78DBAE41-DECE-4E1D-B681-9165169868C6}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{E903C556-8888-4D8C-AFDA-67479295EF1F}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{96D0B5F0-8728-4E41-A67A-B1223FE0E856}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{87DE6BE4-71C9-43EB-B24B-3CA6FFCFD964}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{1488D549-58CC-419C-94D5-6A24C4852E2B}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{C0695BF6-A959-424E-BE48-FC06F9E55ECB}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{EC72B0FF-9461-4F8E-B611-30F8477117E7}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{963741F5-F62A-44B8-BC59-D7B83A975A24}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{2727F537-88C4-4AD9-9430-14D8ED116C9C}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{6154609F-E931-4BE5-B31A-70A67A30A4BA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>